<commit_message>
add excel and begin packaging
</commit_message>
<xml_diff>
--- a/assets/hostel.xlsx
+++ b/assets/hostel.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="January" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="November" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -22,10 +22,34 @@
     <t>Last Name</t>
   </si>
   <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>Nights</t>
+  </si>
+  <si>
     <t>Country</t>
   </si>
   <si>
     <t>Passport #</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>STEF</t>
+  </si>
+  <si>
+    <t>WG</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>69</t>
   </si>
 </sst>
 </file>
@@ -61,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,15 +427,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="32" customWidth="1"/>
-    <col min="4" max="5" width="15" customWidth="1"/>
+    <col min="4" max="5" width="10" customWidth="1"/>
+    <col min="6" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,10 +451,62 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45621</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45621</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
begin adding db function
</commit_message>
<xml_diff>
--- a/assets/hostel.xlsx
+++ b/assets/hostel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -34,22 +34,46 @@
     <t>Passport #</t>
   </si>
   <si>
+    <t>Check Out Date</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Payment Method</t>
+  </si>
+  <si>
+    <t>Amount Paid</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Rooms</t>
+  </si>
+  <si>
+    <t>Beds</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>STEF</t>
+    <t>Stef</t>
   </si>
   <si>
     <t>WG</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
-    <t>69</t>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -427,16 +451,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:P3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="32" customWidth="1"/>
     <col min="4" max="5" width="10" customWidth="1"/>
     <col min="6" max="7" width="15" customWidth="1"/>
+    <col min="8" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="16" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,51 +485,84 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45621</v>
+        <v>45622</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45625</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45621</v>
+        <v>45622</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
+        <v>45625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>